<commit_message>
Adding new link, not inconsistency in spacing and that links are vertically stacked and not tiled.
</commit_message>
<xml_diff>
--- a/LinkDefinitions.xlsx
+++ b/LinkDefinitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\BigPicLinkHTMLGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5B5AF2-F977-48C9-A5FE-67D6F600B7EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B72171E-D319-4DF0-9B68-53C1D5A08A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Label</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>ShangriLaFrontier.png</t>
+  </si>
+  <si>
+    <t>https://www.crunchyroll.com/series/GDKHZEJ0K/solo-leveling</t>
+  </si>
+  <si>
+    <t>Solo Levelling</t>
+  </si>
+  <si>
+    <t>SoloLeveling.jpg</t>
   </si>
 </sst>
 </file>
@@ -371,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,9 +414,21 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{49D53ACB-E36D-43A1-8CA0-5B414DBE79E6}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{018EF221-3983-449B-8D80-E7B86D63EC46}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates with latest shortcuts
</commit_message>
<xml_diff>
--- a/LinkDefinitions.xlsx
+++ b/LinkDefinitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\BigPicLinkHTMLGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8D3759-900E-4AA9-A80B-3C14340FC936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF86A8A-B21D-4DB4-8371-7A19F3C070AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Label</t>
   </si>
@@ -52,6 +52,96 @@
   </si>
   <si>
     <t>SoloLeveling.webp</t>
+  </si>
+  <si>
+    <t>Demon Slayer</t>
+  </si>
+  <si>
+    <t>Hulu</t>
+  </si>
+  <si>
+    <t>Sid the Scientist</t>
+  </si>
+  <si>
+    <t>Daniel Tiger</t>
+  </si>
+  <si>
+    <t>YouTube</t>
+  </si>
+  <si>
+    <t>Free Media Heck Yeah</t>
+  </si>
+  <si>
+    <t>Miruro Anima</t>
+  </si>
+  <si>
+    <t>Pandora</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com</t>
+  </si>
+  <si>
+    <t>https://www.pandora.com</t>
+  </si>
+  <si>
+    <t>https://fmhy.net</t>
+  </si>
+  <si>
+    <t>https://www.miruro.tv</t>
+  </si>
+  <si>
+    <t>https://www.hulu.com/welcome</t>
+  </si>
+  <si>
+    <t>https://www.crunchyroll.com/series/GY5P48XEY/demon-slayer-kimetsu-no-yaiba?srsltid=AfmBOoqt8gh7y_FZv2IkKBba9pTdA26VzePJukANMW2uAR_fGGVYSlk7</t>
+  </si>
+  <si>
+    <t>https://pbskids.org/sid</t>
+  </si>
+  <si>
+    <t>https://pbskids.org/daniel/</t>
+  </si>
+  <si>
+    <t>https://pbskids.org/videos</t>
+  </si>
+  <si>
+    <t>PBS Kids Videos</t>
+  </si>
+  <si>
+    <t>PBS Kids Games</t>
+  </si>
+  <si>
+    <t>https://pbskids.org/games</t>
+  </si>
+  <si>
+    <t>Youtube.jpg</t>
+  </si>
+  <si>
+    <t>miruro-tv-icon.jpg</t>
+  </si>
+  <si>
+    <t>pandora.png</t>
+  </si>
+  <si>
+    <t>DemonSlayer.jpg</t>
+  </si>
+  <si>
+    <t>hulu.jpg</t>
+  </si>
+  <si>
+    <t>Sid.jpg</t>
+  </si>
+  <si>
+    <t>DanielTiger.jpg</t>
+  </si>
+  <si>
+    <t>PBS_Kids_Games.png</t>
+  </si>
+  <si>
+    <t>PBS-Kids-Video.png</t>
+  </si>
+  <si>
+    <t>FMHY.jpeg</t>
   </si>
 </sst>
 </file>
@@ -380,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,30 +495,150 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C7" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{49D53ACB-E36D-43A1-8CA0-5B414DBE79E6}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{018EF221-3983-449B-8D80-E7B86D63EC46}"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{49D53ACB-E36D-43A1-8CA0-5B414DBE79E6}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{018EF221-3983-449B-8D80-E7B86D63EC46}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{74E4A051-CC10-4FFB-861D-5ED4092420CA}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{ECEF39D3-7E3C-41A8-996D-A5BE1F5DB511}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{5333D2D9-7D3D-4693-AE32-39983D6FD673}"/>
+    <hyperlink ref="B5" r:id="rId6" xr:uid="{6E58BDA7-47D7-44B8-8647-94DB74F425BE}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{613DFF9A-5CBA-4719-9071-77042F3491C5}"/>
+    <hyperlink ref="B8" r:id="rId8" xr:uid="{25DEC0DA-9E36-4360-8EDC-8E80DD20A0FB}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{3E938FD6-F01D-448A-AE3C-B0AE9BD9AEC4}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{1F1D45E1-44E6-49CA-964B-974BA3012DD6}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{06BF77CC-EE0D-4802-A1FE-913B40EA57FB}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{2AD069E5-F259-4585-B724-C7E86638CCB7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Replace free media heck yeah with P stream
The AI generated link image is a little funny, but better than the others.
</commit_message>
<xml_diff>
--- a/LinkDefinitions.xlsx
+++ b/LinkDefinitions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\BigPicLinkHTMLGenerator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NetworkShare\BigPicLinkHTMLGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF86A8A-B21D-4DB4-8371-7A19F3C070AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79EA9AF-0086-433C-9DE7-A634AFF6F652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2235" yWindow="390" windowWidth="23985" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>YouTube</t>
   </si>
   <si>
-    <t>Free Media Heck Yeah</t>
-  </si>
-  <si>
     <t>Miruro Anima</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>https://www.pandora.com</t>
   </si>
   <si>
-    <t>https://fmhy.net</t>
-  </si>
-  <si>
     <t>https://www.miruro.tv</t>
   </si>
   <si>
@@ -141,7 +135,13 @@
     <t>PBS-Kids-Video.png</t>
   </si>
   <si>
-    <t>FMHY.jpeg</t>
+    <t>Pstream</t>
+  </si>
+  <si>
+    <t>https://pstream.org/</t>
+  </si>
+  <si>
+    <t>PStream.jpeg</t>
   </si>
 </sst>
 </file>
@@ -472,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,18 +498,18 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
         <v>38</v>
@@ -517,24 +517,24 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -564,10 +564,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -575,10 +575,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -586,10 +586,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -597,32 +597,32 @@
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>